<commit_message>
Add more sound effects, actors and fix some bugs
</commit_message>
<xml_diff>
--- a/Casino/Resources/GameQuestions.xlsx
+++ b/Casino/Resources/GameQuestions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\CasinoGame\Casino\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8670639C-0A9E-49FB-9713-3714F8A06C6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10905783-3C4B-49DF-AF16-5A6533294282}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4575" yWindow="4050" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3855" yWindow="4185" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="139">
   <si>
     <t>Id</t>
   </si>
@@ -205,6 +205,243 @@
   </si>
   <si>
     <t>Grass footsteps</t>
+  </si>
+  <si>
+    <t>حاجة مؤثرة جداً</t>
+  </si>
+  <si>
+    <t>كدة رضا - احمد حلمي</t>
+  </si>
+  <si>
+    <t>يابني ابعد عني يابني</t>
+  </si>
+  <si>
+    <t>الجوكر - محمد صبحي</t>
+  </si>
+  <si>
+    <t>دي حاجة لو عرفتوها تبقوا عُمد</t>
+  </si>
+  <si>
+    <t>محامي خلع - حسن حسني</t>
+  </si>
+  <si>
+    <t>ي س ر ك  ك ر ح ت م</t>
+  </si>
+  <si>
+    <t>كرسي متحرك</t>
+  </si>
+  <si>
+    <t>ة ب ع ل</t>
+  </si>
+  <si>
+    <t>لعبة</t>
+  </si>
+  <si>
+    <t>ة ر ك ف</t>
+  </si>
+  <si>
+    <t xml:space="preserve">فكرة </t>
+  </si>
+  <si>
+    <t>س ي س م ر</t>
+  </si>
+  <si>
+    <t>رمسيس</t>
+  </si>
+  <si>
+    <t>ن و ع ر ف</t>
+  </si>
+  <si>
+    <t>فرعون</t>
+  </si>
+  <si>
+    <t>ل د ا ع  م ا م ا</t>
+  </si>
+  <si>
+    <t>عادل امام</t>
+  </si>
+  <si>
+    <t>ة ع ر ز م  ن ج ا و د</t>
+  </si>
+  <si>
+    <t>ق و ر ش  س م ش ل ا</t>
+  </si>
+  <si>
+    <t>مزرعة دواجن</t>
+  </si>
+  <si>
+    <t>شروق الشمس</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ل ا ي خ</t>
+  </si>
+  <si>
+    <t>ل و ف  س م د م</t>
+  </si>
+  <si>
+    <t>خيال</t>
+  </si>
+  <si>
+    <t>فول مدمس</t>
+  </si>
+  <si>
+    <t>انا بابا يلا</t>
+  </si>
+  <si>
+    <t>تيتو - خالد صالح</t>
+  </si>
+  <si>
+    <t>هنرقص دانص يا روح امك</t>
+  </si>
+  <si>
+    <t>الفرن - عادل ادهم</t>
+  </si>
+  <si>
+    <t>جبت الترنك</t>
+  </si>
+  <si>
+    <t>الناظر - حسين ابو حجاج</t>
+  </si>
+  <si>
+    <t>جي تعزي ولا جي تهزر</t>
+  </si>
+  <si>
+    <t>الكيف - يحيي الفخراني</t>
+  </si>
+  <si>
+    <t>Popcorn</t>
+  </si>
+  <si>
+    <t>Pouring Tea</t>
+  </si>
+  <si>
+    <t>Resources/Soundeffects/popcorn.mp3</t>
+  </si>
+  <si>
+    <t>Resources/Soundeffects/tea.mp3</t>
+  </si>
+  <si>
+    <t>Resources/Soundeffects/thunder.mp3</t>
+  </si>
+  <si>
+    <t>Thunder</t>
+  </si>
+  <si>
+    <t>5 مسلسلات من رمضان 2024</t>
+  </si>
+  <si>
+    <t>بابا جه - الحشاشين - امبراطورية م - عتبات البهجة - مسار اجباري</t>
+  </si>
+  <si>
+    <t>Australia</t>
+  </si>
+  <si>
+    <t>Largest Continet in Area</t>
+  </si>
+  <si>
+    <t>Asia</t>
+  </si>
+  <si>
+    <t>Smallest Continent in Area</t>
+  </si>
+  <si>
+    <t>Country that contains 7000 island</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Phillipins </t>
+  </si>
+  <si>
+    <t>The only Arabic country with no desert</t>
+  </si>
+  <si>
+    <t>Lebanon</t>
+  </si>
+  <si>
+    <t>Who had drawn the Mona Lisa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Leonardo Davinci </t>
+  </si>
+  <si>
+    <t>حاجة بتتاكل عمرها ما بتبوظ</t>
+  </si>
+  <si>
+    <t>العسل</t>
+  </si>
+  <si>
+    <t>اكبر كوكب في المجرة الشمسية؟</t>
+  </si>
+  <si>
+    <t xml:space="preserve">المشترى - Jupiter </t>
+  </si>
+  <si>
+    <t>المغرب في انهي قارة؟</t>
+  </si>
+  <si>
+    <t>افريقيا</t>
+  </si>
+  <si>
+    <t>مين ده؟</t>
+  </si>
+  <si>
+    <t>Tom Hanks</t>
+  </si>
+  <si>
+    <t>Resources/Actors/TomHanks.jpg</t>
+  </si>
+  <si>
+    <t>اكبر عضو في جسم الإنسان؟</t>
+  </si>
+  <si>
+    <t>الجلد</t>
+  </si>
+  <si>
+    <t>علم البرازيل معمول من كام لون؟</t>
+  </si>
+  <si>
+    <t>4 (Yellow, White, Green, Blue)</t>
+  </si>
+  <si>
+    <t>امال لأ امال طبعاً</t>
+  </si>
+  <si>
+    <t>حزمني يا - شريف منير</t>
+  </si>
+  <si>
+    <t>دي اراء ارااااء</t>
+  </si>
+  <si>
+    <t>رمضان مبروك ابو العلمين حمودة - محمد هنيدي</t>
+  </si>
+  <si>
+    <t>انا مش تبع حد انا رئيس جمهورية نفسي</t>
+  </si>
+  <si>
+    <t>ظرف طارق - محمد شرف</t>
+  </si>
+  <si>
+    <t>اغنية للشاب خالد</t>
+  </si>
+  <si>
+    <t>اغنية لـ MTM</t>
+  </si>
+  <si>
+    <t>اغنية لـ وسط البلد</t>
+  </si>
+  <si>
+    <t xml:space="preserve">اغنية لـ شرين </t>
+  </si>
+  <si>
+    <t>اغنية لـ سميرة سعيد</t>
+  </si>
+  <si>
+    <t>اغنية لـ أصالة</t>
+  </si>
+  <si>
+    <t>اغنية لـ محمد هنيدي</t>
+  </si>
+  <si>
+    <t>اغنية لـ حمادة هلال</t>
   </si>
 </sst>
 </file>
@@ -522,17 +759,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E28"/>
+  <dimension ref="A1:E71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" topLeftCell="A59" workbookViewId="0">
+      <selection activeCell="E71" sqref="E71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="58.85546875" customWidth="1"/>
+    <col min="3" max="3" width="35.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="47.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="69.5703125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -694,7 +931,7 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C10" t="s">
         <v>20</v>
@@ -1010,6 +1247,737 @@
       </c>
       <c r="E28" t="s">
         <v>58</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29">
+        <v>6</v>
+      </c>
+      <c r="C29" t="s">
+        <v>60</v>
+      </c>
+      <c r="D29" t="s">
+        <v>61</v>
+      </c>
+      <c r="E29" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30">
+        <v>6</v>
+      </c>
+      <c r="C30" t="s">
+        <v>62</v>
+      </c>
+      <c r="D30" t="s">
+        <v>63</v>
+      </c>
+      <c r="E30" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31">
+        <v>6</v>
+      </c>
+      <c r="C31" t="s">
+        <v>64</v>
+      </c>
+      <c r="D31" t="s">
+        <v>65</v>
+      </c>
+      <c r="E31" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32">
+        <v>2</v>
+      </c>
+      <c r="C32" t="s">
+        <v>66</v>
+      </c>
+      <c r="D32" t="s">
+        <v>67</v>
+      </c>
+      <c r="E32" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33">
+        <v>2</v>
+      </c>
+      <c r="C33" t="s">
+        <v>68</v>
+      </c>
+      <c r="D33" t="s">
+        <v>69</v>
+      </c>
+      <c r="E33" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34">
+        <v>2</v>
+      </c>
+      <c r="C34" t="s">
+        <v>70</v>
+      </c>
+      <c r="D34" t="s">
+        <v>71</v>
+      </c>
+      <c r="E34" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35">
+        <v>2</v>
+      </c>
+      <c r="C35" t="s">
+        <v>72</v>
+      </c>
+      <c r="D35" t="s">
+        <v>73</v>
+      </c>
+      <c r="E35" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36">
+        <v>2</v>
+      </c>
+      <c r="C36" t="s">
+        <v>74</v>
+      </c>
+      <c r="D36" t="s">
+        <v>75</v>
+      </c>
+      <c r="E36" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37">
+        <v>2</v>
+      </c>
+      <c r="C37" t="s">
+        <v>76</v>
+      </c>
+      <c r="D37" t="s">
+        <v>77</v>
+      </c>
+      <c r="E37" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="B38">
+        <v>2</v>
+      </c>
+      <c r="C38" t="s">
+        <v>78</v>
+      </c>
+      <c r="D38" t="s">
+        <v>80</v>
+      </c>
+      <c r="E38" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="B39">
+        <v>2</v>
+      </c>
+      <c r="C39" t="s">
+        <v>79</v>
+      </c>
+      <c r="D39" t="s">
+        <v>81</v>
+      </c>
+      <c r="E39" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="B40">
+        <v>2</v>
+      </c>
+      <c r="C40" t="s">
+        <v>82</v>
+      </c>
+      <c r="D40" t="s">
+        <v>84</v>
+      </c>
+      <c r="E40" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>40</v>
+      </c>
+      <c r="B41">
+        <v>2</v>
+      </c>
+      <c r="C41" t="s">
+        <v>83</v>
+      </c>
+      <c r="D41" t="s">
+        <v>85</v>
+      </c>
+      <c r="E41" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>41</v>
+      </c>
+      <c r="B42">
+        <v>6</v>
+      </c>
+      <c r="C42" t="s">
+        <v>86</v>
+      </c>
+      <c r="D42" t="s">
+        <v>87</v>
+      </c>
+      <c r="E42" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>42</v>
+      </c>
+      <c r="B43">
+        <v>6</v>
+      </c>
+      <c r="C43" t="s">
+        <v>88</v>
+      </c>
+      <c r="D43" t="s">
+        <v>89</v>
+      </c>
+      <c r="E43" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>43</v>
+      </c>
+      <c r="B44">
+        <v>6</v>
+      </c>
+      <c r="C44" t="s">
+        <v>90</v>
+      </c>
+      <c r="D44" t="s">
+        <v>91</v>
+      </c>
+      <c r="E44" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>44</v>
+      </c>
+      <c r="B45">
+        <v>6</v>
+      </c>
+      <c r="C45" t="s">
+        <v>92</v>
+      </c>
+      <c r="D45" t="s">
+        <v>93</v>
+      </c>
+      <c r="E45" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>45</v>
+      </c>
+      <c r="B46">
+        <v>7</v>
+      </c>
+      <c r="C46" t="s">
+        <v>57</v>
+      </c>
+      <c r="D46" t="s">
+        <v>94</v>
+      </c>
+      <c r="E46" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>46</v>
+      </c>
+      <c r="B47">
+        <v>7</v>
+      </c>
+      <c r="C47" t="s">
+        <v>57</v>
+      </c>
+      <c r="D47" t="s">
+        <v>95</v>
+      </c>
+      <c r="E47" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>47</v>
+      </c>
+      <c r="B48">
+        <v>7</v>
+      </c>
+      <c r="C48" t="s">
+        <v>57</v>
+      </c>
+      <c r="D48" t="s">
+        <v>99</v>
+      </c>
+      <c r="E48" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>48</v>
+      </c>
+      <c r="B49">
+        <v>1</v>
+      </c>
+      <c r="C49" t="s">
+        <v>100</v>
+      </c>
+      <c r="D49" t="s">
+        <v>101</v>
+      </c>
+      <c r="E49" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>49</v>
+      </c>
+      <c r="B50">
+        <v>1</v>
+      </c>
+      <c r="C50" t="s">
+        <v>105</v>
+      </c>
+      <c r="D50" t="s">
+        <v>102</v>
+      </c>
+      <c r="E50" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>50</v>
+      </c>
+      <c r="B51">
+        <v>1</v>
+      </c>
+      <c r="C51" t="s">
+        <v>103</v>
+      </c>
+      <c r="D51" t="s">
+        <v>104</v>
+      </c>
+      <c r="E51" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>51</v>
+      </c>
+      <c r="B52">
+        <v>1</v>
+      </c>
+      <c r="C52" t="s">
+        <v>106</v>
+      </c>
+      <c r="D52" t="s">
+        <v>107</v>
+      </c>
+      <c r="E52" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>52</v>
+      </c>
+      <c r="B53">
+        <v>1</v>
+      </c>
+      <c r="C53" t="s">
+        <v>108</v>
+      </c>
+      <c r="D53" t="s">
+        <v>109</v>
+      </c>
+      <c r="E53" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>53</v>
+      </c>
+      <c r="B54">
+        <v>1</v>
+      </c>
+      <c r="C54" t="s">
+        <v>110</v>
+      </c>
+      <c r="D54" t="s">
+        <v>111</v>
+      </c>
+      <c r="E54" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>54</v>
+      </c>
+      <c r="B55">
+        <v>1</v>
+      </c>
+      <c r="C55" t="s">
+        <v>112</v>
+      </c>
+      <c r="D55" t="s">
+        <v>113</v>
+      </c>
+      <c r="E55" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>55</v>
+      </c>
+      <c r="B56">
+        <v>1</v>
+      </c>
+      <c r="C56" t="s">
+        <v>114</v>
+      </c>
+      <c r="D56" t="s">
+        <v>115</v>
+      </c>
+      <c r="E56" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>56</v>
+      </c>
+      <c r="B57">
+        <v>1</v>
+      </c>
+      <c r="C57" t="s">
+        <v>116</v>
+      </c>
+      <c r="D57" t="s">
+        <v>117</v>
+      </c>
+      <c r="E57" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>57</v>
+      </c>
+      <c r="B58">
+        <v>8</v>
+      </c>
+      <c r="C58" t="s">
+        <v>118</v>
+      </c>
+      <c r="D58" t="s">
+        <v>119</v>
+      </c>
+      <c r="E58" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>58</v>
+      </c>
+      <c r="B59">
+        <v>1</v>
+      </c>
+      <c r="C59" t="s">
+        <v>121</v>
+      </c>
+      <c r="D59" t="s">
+        <v>122</v>
+      </c>
+      <c r="E59" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>59</v>
+      </c>
+      <c r="B60">
+        <v>1</v>
+      </c>
+      <c r="C60" t="s">
+        <v>123</v>
+      </c>
+      <c r="D60" t="s">
+        <v>124</v>
+      </c>
+      <c r="E60" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>60</v>
+      </c>
+      <c r="B61">
+        <v>6</v>
+      </c>
+      <c r="C61" t="s">
+        <v>125</v>
+      </c>
+      <c r="D61" t="s">
+        <v>126</v>
+      </c>
+      <c r="E61" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>61</v>
+      </c>
+      <c r="B62">
+        <v>6</v>
+      </c>
+      <c r="C62" t="s">
+        <v>127</v>
+      </c>
+      <c r="D62" t="s">
+        <v>128</v>
+      </c>
+      <c r="E62" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>62</v>
+      </c>
+      <c r="B63">
+        <v>6</v>
+      </c>
+      <c r="C63" t="s">
+        <v>129</v>
+      </c>
+      <c r="D63" t="s">
+        <v>130</v>
+      </c>
+      <c r="E63" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>63</v>
+      </c>
+      <c r="B64">
+        <v>4</v>
+      </c>
+      <c r="C64" t="s">
+        <v>138</v>
+      </c>
+      <c r="D64" t="s">
+        <v>5</v>
+      </c>
+      <c r="E64" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>64</v>
+      </c>
+      <c r="B65">
+        <v>4</v>
+      </c>
+      <c r="C65" t="s">
+        <v>137</v>
+      </c>
+      <c r="D65" t="s">
+        <v>5</v>
+      </c>
+      <c r="E65" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>65</v>
+      </c>
+      <c r="B66">
+        <v>4</v>
+      </c>
+      <c r="C66" t="s">
+        <v>136</v>
+      </c>
+      <c r="D66" t="s">
+        <v>5</v>
+      </c>
+      <c r="E66" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>66</v>
+      </c>
+      <c r="B67">
+        <v>4</v>
+      </c>
+      <c r="C67" t="s">
+        <v>135</v>
+      </c>
+      <c r="D67" t="s">
+        <v>5</v>
+      </c>
+      <c r="E67" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>67</v>
+      </c>
+      <c r="B68">
+        <v>4</v>
+      </c>
+      <c r="C68" t="s">
+        <v>131</v>
+      </c>
+      <c r="D68" t="s">
+        <v>5</v>
+      </c>
+      <c r="E68" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>68</v>
+      </c>
+      <c r="B69">
+        <v>4</v>
+      </c>
+      <c r="C69" t="s">
+        <v>134</v>
+      </c>
+      <c r="D69" t="s">
+        <v>5</v>
+      </c>
+      <c r="E69" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>69</v>
+      </c>
+      <c r="B70">
+        <v>4</v>
+      </c>
+      <c r="C70" t="s">
+        <v>132</v>
+      </c>
+      <c r="D70" t="s">
+        <v>5</v>
+      </c>
+      <c r="E70" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>70</v>
+      </c>
+      <c r="B71">
+        <v>4</v>
+      </c>
+      <c r="C71" t="s">
+        <v>133</v>
+      </c>
+      <c r="D71" t="s">
+        <v>5</v>
+      </c>
+      <c r="E71" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>